<commit_message>
Rwites test results to excel
</commit_message>
<xml_diff>
--- a/Connected Office Web Application/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application/Connected Office Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D_Drawer\Studies\NWU-BSc.IT\Year-3\Semester-2\CMPG323\CMPG323-Project-4-28885198\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D_Drawer\Studies\NWU-BSc.IT\Year-3\Semester-2\CMPG323\CMPG323-Project-4-28885198\Connected Office Web Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8036FB00-157F-43F8-A3C7-279DD21481BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DF34F8-A171-4C7A-80EB-5D476FB15AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24645" yWindow="1215" windowWidth="18000" windowHeight="9480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24990" yWindow="1560" windowWidth="18000" windowHeight="9480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
@@ -1212,7 +1212,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -1280,7 +1280,7 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -1314,7 +1314,7 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
@@ -1348,7 +1348,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>

</xml_diff>